<commit_message>
Revisions from the end of last year + revised notes
</commit_message>
<xml_diff>
--- a/CS297-WeeklyIndividualReport.xlsx
+++ b/CS297-WeeklyIndividualReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS297-CourseMaterials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC67445B-EC99-B446-BEE1-07B56080ECC0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD1E628D-F523-1C47-92D4-661D981C47C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="500" windowWidth="20420" windowHeight="14640" xr2:uid="{AF13BEBC-A70C-7746-A217-C0986067414B}"/>
+    <workbookView xWindow="80" yWindow="500" windowWidth="20420" windowHeight="14600" activeTab="3" xr2:uid="{AF13BEBC-A70C-7746-A217-C0986067414B}"/>
   </bookViews>
   <sheets>
     <sheet name="Attendence" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="User Stories" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -130,9 +129,6 @@
     <t>PRs</t>
   </si>
   <si>
-    <t>Number of task or user story hours completed each week</t>
-  </si>
-  <si>
     <t>Hours</t>
   </si>
   <si>
@@ -146,6 +142,9 @@
   </si>
   <si>
     <t>Overall Total</t>
+  </si>
+  <si>
+    <t>Story points (or hours) completed each week</t>
   </si>
 </sst>
 </file>
@@ -625,7 +624,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -735,7 +734,7 @@
       <c r="M4" s="9"/>
       <c r="N4" s="9"/>
       <c r="O4" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
@@ -1023,7 +1022,7 @@
       </c>
       <c r="C19" s="10"/>
       <c r="M19" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O19">
         <f>SUM(O5:O17)</f>
@@ -1080,7 +1079,7 @@
   <sheetData>
     <row r="1" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:61" x14ac:dyDescent="0.2">
@@ -1179,7 +1178,7 @@
         <v>4</v>
       </c>
       <c r="F3" s="23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G3" s="26" t="s">
         <v>1</v>
@@ -1194,7 +1193,7 @@
         <v>4</v>
       </c>
       <c r="K3" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L3" s="25" t="s">
         <v>1</v>
@@ -1209,7 +1208,7 @@
         <v>4</v>
       </c>
       <c r="P3" s="23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Q3" s="26" t="s">
         <v>1</v>
@@ -1224,7 +1223,7 @@
         <v>4</v>
       </c>
       <c r="U3" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="V3" s="23" t="s">
         <v>1</v>
@@ -1239,7 +1238,7 @@
         <v>4</v>
       </c>
       <c r="Z3" s="23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AA3" s="28" t="s">
         <v>1</v>
@@ -1254,7 +1253,7 @@
         <v>4</v>
       </c>
       <c r="AE3" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AF3" s="23" t="s">
         <v>1</v>
@@ -1269,7 +1268,7 @@
         <v>4</v>
       </c>
       <c r="AJ3" s="23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AK3" s="26" t="s">
         <v>1</v>
@@ -1284,7 +1283,7 @@
         <v>4</v>
       </c>
       <c r="AO3" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AP3" s="23" t="s">
         <v>1</v>
@@ -1299,7 +1298,7 @@
         <v>4</v>
       </c>
       <c r="AT3" s="23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AU3" s="26" t="s">
         <v>1</v>
@@ -1314,7 +1313,7 @@
         <v>4</v>
       </c>
       <c r="AY3" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AZ3" s="9"/>
       <c r="BA3" s="8"/>
@@ -1551,9 +1550,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1562,7 +1559,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -1599,7 +1596,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" s="21"/>
       <c r="C3" s="22"/>

</xml_diff>

<commit_message>
Making additions to the progress report spreadsheet
</commit_message>
<xml_diff>
--- a/CS297-WeeklyIndividualReport.xlsx
+++ b/CS297-WeeklyIndividualReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS297-CourseMaterials/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birdb/Projects/CS297-Repos/CS297-CourseMaterials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1F91118-0465-A44D-8316-68D1AD30C6EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{717B4EF1-1D98-BA46-BAF4-7F038D53355B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="26240" windowHeight="15480" xr2:uid="{AF13BEBC-A70C-7746-A217-C0986067414B}"/>
+    <workbookView xWindow="13120" yWindow="1700" windowWidth="26240" windowHeight="15480" activeTab="1" xr2:uid="{AF13BEBC-A70C-7746-A217-C0986067414B}"/>
   </bookViews>
   <sheets>
     <sheet name="Attendence" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="49">
   <si>
     <t>Week 1</t>
   </si>
@@ -152,13 +152,40 @@
     <t>Number of PRs created per week</t>
   </si>
   <si>
-    <t>Number of task or user story points completed each week</t>
-  </si>
-  <si>
     <t>CS297 Capstone, spring 2025</t>
   </si>
   <si>
     <t>Subtotal</t>
+  </si>
+  <si>
+    <t>GitHub</t>
+  </si>
+  <si>
+    <t>Jira</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>No meeting</t>
+  </si>
+  <si>
+    <t>Number of task user story points completed each week</t>
+  </si>
+  <si>
+    <t>Is your work up to date on Jira?</t>
+  </si>
+  <si>
+    <t>Is anything hindering your work?</t>
+  </si>
+  <si>
+    <t>Is all your code pushed to your branch on GitHub?</t>
+  </si>
+  <si>
+    <t>Is there anything you need help with?</t>
+  </si>
+  <si>
+    <t>What is your assessment of your progress this week?</t>
   </si>
 </sst>
 </file>
@@ -203,7 +230,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -264,8 +291,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -301,11 +334,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </left>
+      <right style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -352,17 +407,47 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -679,10 +764,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ECC46A0-6323-9B42-9B37-FFE0E0EE37C2}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Q22"/>
+  <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G29" sqref="F29:G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -695,56 +780,27 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="34" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="35" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="35" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" s="6"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="45"/>
+      <c r="F2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
@@ -756,16 +812,17 @@
       <c r="Q2" s="3"/>
     </row>
     <row r="3" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="45"/>
+      <c r="F3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
@@ -777,74 +834,90 @@
       <c r="Q3" s="3"/>
     </row>
     <row r="4" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
+      <c r="A4" s="31"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="38"/>
       <c r="N4" s="6"/>
-      <c r="O4" s="3" t="s">
-        <v>33</v>
-      </c>
+      <c r="O4" s="3"/>
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
     </row>
-    <row r="5" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="17" t="s">
+    <row r="5" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D5" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="41" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="42" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="42" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5" s="42" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5" s="42" t="s">
+        <v>12</v>
+      </c>
+      <c r="M5" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="N5" s="6"/>
+      <c r="O5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+    </row>
+    <row r="6" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="31">
-        <f>COUNTIF(D5:M5, "P") + ROUND(0.7*COUNTIF(D5:M5, "L"),0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="39"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="29">
+        <f>COUNTIF(D6:M6, "P") + ROUND(0.7*COUNTIF(D6:M6, "L"),0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="20">
+      <c r="B7" s="20">
         <v>1</v>
-      </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="31">
-        <f t="shared" ref="O6:O17" si="0">COUNTIF(D6:M6, "P") + ROUND(0.7*COUNTIF(D6:M6, "L"),0)</f>
-        <v>0</v>
-      </c>
-      <c r="P6" s="32"/>
-    </row>
-    <row r="7" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="19"/>
-      <c r="B7" s="20">
-        <v>2</v>
       </c>
       <c r="C7" s="20"/>
       <c r="D7" s="9"/>
@@ -858,15 +931,16 @@
       <c r="L7" s="9"/>
       <c r="M7" s="9"/>
       <c r="N7" s="11"/>
-      <c r="O7" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="O7" s="29">
+        <f t="shared" ref="O7:O18" si="0">COUNTIF(D7:M7, "P") + ROUND(0.7*COUNTIF(D7:M7, "L"),0)</f>
+        <v>0</v>
+      </c>
+      <c r="P7" s="30"/>
     </row>
     <row r="8" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="19"/>
       <c r="B8" s="20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" s="20"/>
       <c r="D8" s="9"/>
@@ -880,7 +954,7 @@
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
       <c r="N8" s="11"/>
-      <c r="O8" s="31">
+      <c r="O8" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -888,7 +962,7 @@
     <row r="9" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="19"/>
       <c r="B9" s="20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C9" s="20"/>
       <c r="D9" s="9"/>
@@ -902,7 +976,7 @@
       <c r="L9" s="9"/>
       <c r="M9" s="9"/>
       <c r="N9" s="11"/>
-      <c r="O9" s="31">
+      <c r="O9" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -910,7 +984,7 @@
     <row r="10" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="19"/>
       <c r="B10" s="20">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" s="20"/>
       <c r="D10" s="9"/>
@@ -924,39 +998,39 @@
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
       <c r="N10" s="11"/>
-      <c r="O10" s="31">
+      <c r="O10" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="19"/>
+      <c r="B11" s="20">
+        <v>5</v>
+      </c>
+      <c r="C11" s="20"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="18">
+      <c r="B12" s="18">
         <v>1</v>
-      </c>
-      <c r="C11" s="18"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="11"/>
-      <c r="O11" s="31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="17"/>
-      <c r="B12" s="18">
-        <v>2</v>
       </c>
       <c r="C12" s="18"/>
       <c r="D12" s="8"/>
@@ -970,7 +1044,7 @@
       <c r="L12" s="8"/>
       <c r="M12" s="8"/>
       <c r="N12" s="11"/>
-      <c r="O12" s="31">
+      <c r="O12" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -978,7 +1052,7 @@
     <row r="13" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="17"/>
       <c r="B13" s="18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="8"/>
@@ -992,7 +1066,7 @@
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>
       <c r="N13" s="11"/>
-      <c r="O13" s="31">
+      <c r="O13" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1000,7 +1074,7 @@
     <row r="14" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="17"/>
       <c r="B14" s="18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C14" s="18"/>
       <c r="D14" s="8"/>
@@ -1014,7 +1088,7 @@
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
       <c r="N14" s="11"/>
-      <c r="O14" s="31">
+      <c r="O14" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1022,7 +1096,7 @@
     <row r="15" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="17"/>
       <c r="B15" s="18">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C15" s="18"/>
       <c r="D15" s="8"/>
@@ -1036,96 +1110,126 @@
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
       <c r="N15" s="11"/>
-      <c r="O15" s="31">
+      <c r="O15" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="17"/>
+      <c r="B16" s="18">
+        <v>5</v>
+      </c>
+      <c r="C16" s="18"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="11"/>
-      <c r="O16" s="31">
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="17" t="s">
+    <row r="18" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="11"/>
-      <c r="O17" s="31">
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B19" s="1" t="s">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="M19" s="1" t="s">
+      <c r="C20" s="1"/>
+      <c r="M20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O19" s="16">
-        <f>SUM(O5:O17)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" t="s">
-        <v>15</v>
+      <c r="O20" s="16">
+        <f>SUM(O6:O18)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
         <v>19</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D23" t="s">
         <v>20</v>
       </c>
     </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B17">
-    <sortCondition ref="A2:A17"/>
-    <sortCondition ref="B2:B17"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B18">
+    <sortCondition ref="A2:A18"/>
+    <sortCondition ref="B2:B18"/>
   </sortState>
   <mergeCells count="2">
     <mergeCell ref="B2:C2"/>
@@ -1140,8 +1244,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:BI26"/>
   <sheetViews>
-    <sheetView zoomScale="99" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1465,7 +1569,7 @@
     </row>
     <row r="5" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" s="11"/>
       <c r="C5" s="14"/>
@@ -1556,67 +1660,85 @@
         <f>SUM(B4:AY4)</f>
         <v>0</v>
       </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="30"/>
-      <c r="J6" s="30"/>
-      <c r="K6" s="30"/>
-      <c r="L6" s="30"/>
-      <c r="M6" s="30"/>
-      <c r="N6" s="30"/>
-      <c r="O6" s="30"/>
-      <c r="P6" s="30"/>
-      <c r="Q6" s="30"/>
-      <c r="R6" s="30"/>
-      <c r="S6" s="30"/>
-      <c r="T6" s="30"/>
-      <c r="U6" s="30"/>
-      <c r="V6" s="30"/>
-      <c r="W6" s="30"/>
-      <c r="X6" s="30"/>
-      <c r="Y6" s="30"/>
-      <c r="Z6" s="30"/>
-      <c r="AA6" s="30"/>
-      <c r="AB6" s="30"/>
-      <c r="AC6" s="30"/>
-      <c r="AD6" s="30"/>
-      <c r="AE6" s="30"/>
-      <c r="AF6" s="30"/>
-      <c r="AG6" s="30"/>
-      <c r="AH6" s="30"/>
-      <c r="AI6" s="30"/>
-      <c r="AJ6" s="30"/>
-      <c r="AK6" s="30"/>
-      <c r="AL6" s="30"/>
-      <c r="AM6" s="30"/>
-      <c r="AN6" s="30"/>
-      <c r="AO6" s="30"/>
-      <c r="AP6" s="30"/>
-      <c r="AQ6" s="30"/>
-      <c r="AR6" s="30"/>
-      <c r="AS6" s="30"/>
-      <c r="AT6" s="30"/>
-      <c r="AU6" s="30"/>
-      <c r="AV6" s="30"/>
-      <c r="AW6" s="30"/>
-      <c r="AX6" s="30"/>
-      <c r="AY6" s="30"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="28"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="28"/>
+      <c r="O6" s="28"/>
+      <c r="P6" s="28"/>
+      <c r="Q6" s="28"/>
+      <c r="R6" s="28"/>
+      <c r="S6" s="28"/>
+      <c r="T6" s="28"/>
+      <c r="U6" s="28"/>
+      <c r="V6" s="28"/>
+      <c r="W6" s="28"/>
+      <c r="X6" s="28"/>
+      <c r="Y6" s="28"/>
+      <c r="Z6" s="28"/>
+      <c r="AA6" s="28"/>
+      <c r="AB6" s="28"/>
+      <c r="AC6" s="28"/>
+      <c r="AD6" s="28"/>
+      <c r="AE6" s="28"/>
+      <c r="AF6" s="28"/>
+      <c r="AG6" s="28"/>
+      <c r="AH6" s="28"/>
+      <c r="AI6" s="28"/>
+      <c r="AJ6" s="28"/>
+      <c r="AK6" s="28"/>
+      <c r="AL6" s="28"/>
+      <c r="AM6" s="28"/>
+      <c r="AN6" s="28"/>
+      <c r="AO6" s="28"/>
+      <c r="AP6" s="28"/>
+      <c r="AQ6" s="28"/>
+      <c r="AR6" s="28"/>
+      <c r="AS6" s="28"/>
+      <c r="AT6" s="28"/>
+      <c r="AU6" s="28"/>
+      <c r="AV6" s="28"/>
+      <c r="AW6" s="28"/>
+      <c r="AX6" s="28"/>
+      <c r="AY6" s="28"/>
     </row>
     <row r="8" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="B8" s="7"/>
+      <c r="A8" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="47"/>
     </row>
     <row r="9" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="B9" s="7"/>
+      <c r="A9" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="47"/>
     </row>
     <row r="10" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="B10" s="7"/>
+      <c r="A10" s="46" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="48"/>
     </row>
     <row r="11" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="B11" s="7"/>
+      <c r="A11" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="47"/>
+    </row>
+    <row r="12" spans="1:61" x14ac:dyDescent="0.2">
+      <c r="A12" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="49"/>
     </row>
     <row r="13" spans="1:61" x14ac:dyDescent="0.2">
       <c r="B13" s="7"/>
@@ -1652,6 +1774,13 @@
       <c r="B26" s="7"/>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1662,7 +1791,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1705,7 +1834,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="31" t="s">
         <v>30</v>
       </c>
       <c r="B3" s="12"/>
@@ -1733,7 +1862,7 @@
       <c r="K4" s="14"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="31" t="s">
         <v>29</v>
       </c>
       <c r="B5" s="27">
@@ -1752,7 +1881,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1762,7 +1891,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -1798,7 +1927,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="31" t="s">
         <v>31</v>
       </c>
       <c r="B3" s="12"/>
@@ -1826,7 +1955,7 @@
       <c r="K4" s="14"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="31" t="s">
         <v>29</v>
       </c>
       <c r="B5" s="27">

</xml_diff>

<commit_message>
Additions to the template workbook
</commit_message>
<xml_diff>
--- a/CS297-WeeklyIndividualReport.xlsx
+++ b/CS297-WeeklyIndividualReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/birdb/Projects/CS297-Repos/CS297-CourseMaterials/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS297-CourseMaterials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{717B4EF1-1D98-BA46-BAF4-7F038D53355B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61971F4C-094F-BA44-918F-38B1BC66FC5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13120" yWindow="1700" windowWidth="26240" windowHeight="15480" activeTab="1" xr2:uid="{AF13BEBC-A70C-7746-A217-C0986067414B}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="26240" windowHeight="15500" xr2:uid="{AF13BEBC-A70C-7746-A217-C0986067414B}"/>
   </bookViews>
   <sheets>
     <sheet name="Attendence" sheetId="1" r:id="rId1"/>
@@ -192,7 +192,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -210,13 +210,6 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -281,12 +274,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -297,8 +284,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -349,8 +342,163 @@
     </border>
     <border>
       <left/>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </left>
+      <right style="hair">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </left>
+      <right style="hair">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
-        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
       </right>
       <top/>
       <bottom/>
@@ -360,10 +508,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -377,7 +524,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -407,48 +554,74 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -766,8 +939,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="F29:G29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -783,400 +956,393 @@
         <v>37</v>
       </c>
       <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="D1" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="35"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" s="38"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="36"/>
     </row>
     <row r="2" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="45"/>
-      <c r="F2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
+      <c r="A2" s="49"/>
+      <c r="D2" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="37"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="I2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" s="38"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="36"/>
+      <c r="Q2" s="2"/>
     </row>
     <row r="3" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="45"/>
-      <c r="F3" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
+      <c r="A3" s="50"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
     </row>
     <row r="4" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="31"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
-      <c r="K4" s="38"/>
-      <c r="L4" s="38"/>
-      <c r="M4" s="38"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
+      <c r="A4" s="51"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="44"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
     </row>
     <row r="5" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D5" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="41" t="s">
+      <c r="A5" s="52"/>
+      <c r="D5" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="42" t="s">
+      <c r="F5" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="42" t="s">
+      <c r="G5" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="42" t="s">
+      <c r="H5" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="42" t="s">
+      <c r="I5" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="42" t="s">
+      <c r="J5" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="42" t="s">
+      <c r="K5" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="42" t="s">
+      <c r="L5" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="42" t="s">
+      <c r="M5" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="6"/>
-      <c r="O5" s="3" t="s">
+      <c r="N5" s="5"/>
+      <c r="O5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-    </row>
-    <row r="6" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+    </row>
+    <row r="6" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="40"/>
-      <c r="L6" s="39"/>
-      <c r="M6" s="40"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="29">
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="31"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="53">
         <f>COUNTIF(D6:M6, "P") + ROUND(0.7*COUNTIF(D6:M6, "L"),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="19" t="s">
+    <row r="7" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="20">
+      <c r="B7" s="19">
         <v>1</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="29">
+      <c r="C7" s="19"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="53">
         <f t="shared" ref="O7:O18" si="0">COUNTIF(D7:M7, "P") + ROUND(0.7*COUNTIF(D7:M7, "L"),0)</f>
         <v>0</v>
       </c>
-      <c r="P7" s="30"/>
-    </row>
-    <row r="8" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="19"/>
-      <c r="B8" s="20">
+      <c r="P7" s="27"/>
+    </row>
+    <row r="8" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="18"/>
+      <c r="B8" s="19">
         <v>2</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="29">
+      <c r="C8" s="19"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="53">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="19"/>
-      <c r="B9" s="20">
+    <row r="9" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="18"/>
+      <c r="B9" s="19">
         <v>3</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="29">
+      <c r="C9" s="19"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="53">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="19"/>
-      <c r="B10" s="20">
+    <row r="10" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="18"/>
+      <c r="B10" s="19">
         <v>4</v>
       </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="29">
+      <c r="C10" s="19"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="53">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="19"/>
-      <c r="B11" s="20">
+    <row r="11" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="18"/>
+      <c r="B11" s="19">
         <v>5</v>
       </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="11"/>
-      <c r="O11" s="29">
+      <c r="C11" s="19"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="53">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="17" t="s">
+    <row r="12" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="18">
+      <c r="B12" s="17">
         <v>1</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="11"/>
-      <c r="O12" s="29">
+      <c r="C12" s="17"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="53">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="17"/>
-      <c r="B13" s="18">
+    <row r="13" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="16"/>
+      <c r="B13" s="17">
         <v>2</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="11"/>
-      <c r="O13" s="29">
+      <c r="C13" s="17"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="53">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="17"/>
-      <c r="B14" s="18">
+    <row r="14" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="16"/>
+      <c r="B14" s="17">
         <v>3</v>
       </c>
-      <c r="C14" s="18"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="11"/>
-      <c r="O14" s="29">
+      <c r="C14" s="17"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="53">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="17"/>
-      <c r="B15" s="18">
+    <row r="15" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="16"/>
+      <c r="B15" s="17">
         <v>4</v>
       </c>
-      <c r="C15" s="18"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="29">
+      <c r="C15" s="17"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="53">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="17"/>
-      <c r="B16" s="18">
+    <row r="16" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="16"/>
+      <c r="B16" s="17">
         <v>5</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="11"/>
-      <c r="O16" s="29">
+      <c r="C16" s="17"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="53">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="19" t="s">
+    <row r="17" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="11"/>
-      <c r="O17" s="29">
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="53">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="17" t="s">
+    <row r="18" spans="1:15" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="11"/>
-      <c r="O18" s="29">
+      <c r="B18" s="17"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="53">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1189,7 +1355,7 @@
       <c r="M20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="O20" s="16">
+      <c r="O20" s="15">
         <f>SUM(O6:O18)</f>
         <v>0</v>
       </c>
@@ -1231,9 +1397,11 @@
     <sortCondition ref="A2:A18"/>
     <sortCondition ref="B2:B18"/>
   </sortState>
-  <mergeCells count="2">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
+  <mergeCells count="4">
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="J2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1244,8 +1412,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:BI26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD12"/>
+    <sheetView zoomScale="99" workbookViewId="0">
+      <selection activeCell="AQ19" sqref="AQ19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1259,395 +1427,395 @@
       </c>
     </row>
     <row r="2" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="B2" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="24" t="s">
+      <c r="B2" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="23" t="s">
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="23"/>
-      <c r="Q2" s="24" t="s">
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="R2" s="25"/>
-      <c r="S2" s="25"/>
-      <c r="T2" s="25"/>
-      <c r="U2" s="25"/>
-      <c r="V2" s="21" t="s">
+      <c r="R2" s="24"/>
+      <c r="S2" s="24"/>
+      <c r="T2" s="24"/>
+      <c r="U2" s="24"/>
+      <c r="V2" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="W2" s="22"/>
-      <c r="X2" s="22"/>
-      <c r="Y2" s="22"/>
-      <c r="Z2" s="22"/>
-      <c r="AA2" s="26" t="s">
+      <c r="W2" s="21"/>
+      <c r="X2" s="21"/>
+      <c r="Y2" s="21"/>
+      <c r="Z2" s="21"/>
+      <c r="AA2" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="AB2" s="26"/>
-      <c r="AC2" s="26"/>
-      <c r="AD2" s="26"/>
-      <c r="AE2" s="26"/>
-      <c r="AF2" s="21" t="s">
+      <c r="AB2" s="25"/>
+      <c r="AC2" s="25"/>
+      <c r="AD2" s="25"/>
+      <c r="AE2" s="25"/>
+      <c r="AF2" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="AG2" s="22"/>
-      <c r="AH2" s="22"/>
-      <c r="AI2" s="22"/>
-      <c r="AJ2" s="22"/>
-      <c r="AK2" s="24" t="s">
+      <c r="AG2" s="21"/>
+      <c r="AH2" s="21"/>
+      <c r="AI2" s="21"/>
+      <c r="AJ2" s="21"/>
+      <c r="AK2" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="AL2" s="24"/>
-      <c r="AM2" s="24"/>
-      <c r="AN2" s="24"/>
-      <c r="AO2" s="24"/>
-      <c r="AP2" s="21" t="s">
+      <c r="AL2" s="23"/>
+      <c r="AM2" s="23"/>
+      <c r="AN2" s="23"/>
+      <c r="AO2" s="23"/>
+      <c r="AP2" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="AQ2" s="22"/>
-      <c r="AR2" s="22"/>
-      <c r="AS2" s="22"/>
-      <c r="AT2" s="22"/>
-      <c r="AU2" s="24" t="s">
+      <c r="AQ2" s="21"/>
+      <c r="AR2" s="21"/>
+      <c r="AS2" s="21"/>
+      <c r="AT2" s="21"/>
+      <c r="AU2" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="AV2" s="25"/>
-      <c r="AW2" s="25"/>
-      <c r="AX2" s="25"/>
-      <c r="AY2" s="25"/>
-      <c r="AZ2" s="6"/>
-      <c r="BA2" s="4"/>
-      <c r="BB2" s="5"/>
-      <c r="BC2" s="5"/>
-      <c r="BD2" s="5"/>
-      <c r="BE2" s="4"/>
-      <c r="BF2" s="4"/>
-      <c r="BG2" s="5"/>
-      <c r="BH2" s="5"/>
-      <c r="BI2" s="5"/>
+      <c r="AV2" s="24"/>
+      <c r="AW2" s="24"/>
+      <c r="AX2" s="24"/>
+      <c r="AY2" s="24"/>
+      <c r="AZ2" s="5"/>
+      <c r="BA2" s="3"/>
+      <c r="BB2" s="4"/>
+      <c r="BC2" s="4"/>
+      <c r="BD2" s="4"/>
+      <c r="BE2" s="3"/>
+      <c r="BF2" s="3"/>
+      <c r="BG2" s="4"/>
+      <c r="BH2" s="4"/>
+      <c r="BI2" s="4"/>
     </row>
     <row r="3" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="24" t="s">
+      <c r="I3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="24" t="s">
+      <c r="J3" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="24" t="s">
+      <c r="K3" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="23" t="s">
+      <c r="L3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="M3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="N3" s="21" t="s">
+      <c r="N3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="21" t="s">
+      <c r="O3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="P3" s="21" t="s">
+      <c r="P3" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="Q3" s="24" t="s">
+      <c r="Q3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="R3" s="24" t="s">
+      <c r="R3" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="S3" s="24" t="s">
+      <c r="S3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="T3" s="24" t="s">
+      <c r="T3" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="U3" s="24" t="s">
+      <c r="U3" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="V3" s="21" t="s">
+      <c r="V3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="W3" s="21" t="s">
+      <c r="W3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="X3" s="21" t="s">
+      <c r="X3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="Y3" s="21" t="s">
+      <c r="Y3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="Z3" s="21" t="s">
+      <c r="Z3" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="AA3" s="26" t="s">
+      <c r="AA3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="AB3" s="24" t="s">
+      <c r="AB3" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="AC3" s="24" t="s">
+      <c r="AC3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="AD3" s="24" t="s">
+      <c r="AD3" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="AE3" s="24" t="s">
+      <c r="AE3" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="AF3" s="21" t="s">
+      <c r="AF3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="AG3" s="21" t="s">
+      <c r="AG3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="AH3" s="21" t="s">
+      <c r="AH3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="AI3" s="21" t="s">
+      <c r="AI3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="AJ3" s="21" t="s">
+      <c r="AJ3" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="AK3" s="24" t="s">
+      <c r="AK3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="AL3" s="24" t="s">
+      <c r="AL3" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="AM3" s="24" t="s">
+      <c r="AM3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="AN3" s="24" t="s">
+      <c r="AN3" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="AO3" s="24" t="s">
+      <c r="AO3" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="AP3" s="21" t="s">
+      <c r="AP3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="AQ3" s="21" t="s">
+      <c r="AQ3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="AR3" s="21" t="s">
+      <c r="AR3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="AS3" s="21" t="s">
+      <c r="AS3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="AT3" s="21" t="s">
+      <c r="AT3" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="AU3" s="24" t="s">
+      <c r="AU3" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="AV3" s="24" t="s">
+      <c r="AV3" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="AW3" s="24" t="s">
+      <c r="AW3" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="AX3" s="24" t="s">
+      <c r="AX3" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="AY3" s="24" t="s">
+      <c r="AY3" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="AZ3" s="6"/>
-      <c r="BA3" s="4"/>
-      <c r="BB3" s="4"/>
-      <c r="BC3" s="4"/>
-      <c r="BD3" s="4"/>
-      <c r="BE3" s="4"/>
-      <c r="BF3" s="4"/>
-      <c r="BG3" s="4"/>
-      <c r="BH3" s="4"/>
-      <c r="BI3" s="4"/>
+      <c r="AZ3" s="5"/>
+      <c r="BA3" s="3"/>
+      <c r="BB3" s="3"/>
+      <c r="BC3" s="3"/>
+      <c r="BD3" s="3"/>
+      <c r="BE3" s="3"/>
+      <c r="BF3" s="3"/>
+      <c r="BG3" s="3"/>
+      <c r="BH3" s="3"/>
+      <c r="BI3" s="3"/>
     </row>
     <row r="4" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="9"/>
-      <c r="U4" s="9"/>
-      <c r="V4" s="8"/>
-      <c r="W4" s="8"/>
-      <c r="X4" s="8"/>
-      <c r="Y4" s="8"/>
-      <c r="Z4" s="8"/>
-      <c r="AA4" s="9"/>
-      <c r="AB4" s="9"/>
-      <c r="AC4" s="9"/>
-      <c r="AD4" s="9"/>
-      <c r="AE4" s="9"/>
-      <c r="AF4" s="8"/>
-      <c r="AG4" s="8"/>
-      <c r="AH4" s="8"/>
-      <c r="AI4" s="8"/>
-      <c r="AJ4" s="8"/>
-      <c r="AK4" s="9"/>
-      <c r="AL4" s="9"/>
-      <c r="AM4" s="9"/>
-      <c r="AN4" s="9"/>
-      <c r="AO4" s="9"/>
-      <c r="AP4" s="8"/>
-      <c r="AQ4" s="8"/>
-      <c r="AR4" s="8"/>
-      <c r="AS4" s="8"/>
-      <c r="AT4" s="8"/>
-      <c r="AU4" s="9"/>
-      <c r="AV4" s="9"/>
-      <c r="AW4" s="9"/>
-      <c r="AX4" s="9"/>
-      <c r="AY4" s="9"/>
-      <c r="AZ4" s="7"/>
-      <c r="BA4" s="7"/>
-      <c r="BB4" s="7"/>
-      <c r="BC4" s="7"/>
-      <c r="BD4" s="7"/>
-      <c r="BE4" s="7"/>
-      <c r="BF4" s="7"/>
-      <c r="BG4" s="7"/>
-      <c r="BH4" s="7"/>
-      <c r="BI4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="7"/>
+      <c r="Z4" s="7"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
+      <c r="AC4" s="8"/>
+      <c r="AD4" s="8"/>
+      <c r="AE4" s="8"/>
+      <c r="AF4" s="7"/>
+      <c r="AG4" s="7"/>
+      <c r="AH4" s="7"/>
+      <c r="AI4" s="7"/>
+      <c r="AJ4" s="7"/>
+      <c r="AK4" s="8"/>
+      <c r="AL4" s="8"/>
+      <c r="AM4" s="8"/>
+      <c r="AN4" s="8"/>
+      <c r="AO4" s="8"/>
+      <c r="AP4" s="7"/>
+      <c r="AQ4" s="7"/>
+      <c r="AR4" s="7"/>
+      <c r="AS4" s="7"/>
+      <c r="AT4" s="7"/>
+      <c r="AU4" s="8"/>
+      <c r="AV4" s="8"/>
+      <c r="AW4" s="8"/>
+      <c r="AX4" s="8"/>
+      <c r="AY4" s="8"/>
+      <c r="AZ4" s="6"/>
+      <c r="BA4" s="6"/>
+      <c r="BB4" s="6"/>
+      <c r="BC4" s="6"/>
+      <c r="BD4" s="6"/>
+      <c r="BE4" s="6"/>
+      <c r="BF4" s="6"/>
+      <c r="BG4" s="6"/>
+      <c r="BH4" s="6"/>
+      <c r="BI4" s="6"/>
     </row>
     <row r="5" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="16">
+      <c r="B5" s="10"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="15">
         <f>SUM(B4:F4)</f>
         <v>0</v>
       </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="16">
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="15">
         <f>SUM(G4:K4)</f>
         <v>0</v>
       </c>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="16">
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="15">
         <f>SUM(L4:P4)</f>
         <v>0</v>
       </c>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="14"/>
-      <c r="S5" s="14"/>
-      <c r="T5" s="14"/>
-      <c r="U5" s="16">
+      <c r="Q5" s="13"/>
+      <c r="R5" s="13"/>
+      <c r="S5" s="13"/>
+      <c r="T5" s="13"/>
+      <c r="U5" s="15">
         <f>SUM(Q4:U4)</f>
         <v>0</v>
       </c>
-      <c r="V5" s="14"/>
-      <c r="W5" s="14"/>
-      <c r="X5" s="14"/>
-      <c r="Y5" s="14"/>
-      <c r="Z5" s="16">
+      <c r="V5" s="13"/>
+      <c r="W5" s="13"/>
+      <c r="X5" s="13"/>
+      <c r="Y5" s="13"/>
+      <c r="Z5" s="15">
         <f>SUM(V4:Z4)</f>
         <v>0</v>
       </c>
-      <c r="AA5" s="14"/>
-      <c r="AB5" s="14"/>
-      <c r="AC5" s="14"/>
-      <c r="AD5" s="14"/>
-      <c r="AE5" s="16">
+      <c r="AA5" s="13"/>
+      <c r="AB5" s="13"/>
+      <c r="AC5" s="13"/>
+      <c r="AD5" s="13"/>
+      <c r="AE5" s="15">
         <f>SUM(AA4:AE4)</f>
         <v>0</v>
       </c>
-      <c r="AF5" s="14"/>
-      <c r="AG5" s="14"/>
-      <c r="AH5" s="14"/>
-      <c r="AI5" s="14"/>
-      <c r="AJ5" s="16">
+      <c r="AF5" s="13"/>
+      <c r="AG5" s="13"/>
+      <c r="AH5" s="13"/>
+      <c r="AI5" s="13"/>
+      <c r="AJ5" s="15">
         <f>SUM(AF4:AJ4)</f>
         <v>0</v>
       </c>
-      <c r="AK5" s="14"/>
-      <c r="AL5" s="14"/>
-      <c r="AM5" s="14"/>
-      <c r="AN5" s="14"/>
-      <c r="AO5" s="16">
+      <c r="AK5" s="13"/>
+      <c r="AL5" s="13"/>
+      <c r="AM5" s="13"/>
+      <c r="AN5" s="13"/>
+      <c r="AO5" s="15">
         <f>SUM(AK4:AO4)</f>
         <v>0</v>
       </c>
-      <c r="AP5" s="14"/>
-      <c r="AQ5" s="14"/>
-      <c r="AR5" s="14"/>
-      <c r="AS5" s="14"/>
-      <c r="AT5" s="16">
+      <c r="AP5" s="13"/>
+      <c r="AQ5" s="13"/>
+      <c r="AR5" s="13"/>
+      <c r="AS5" s="13"/>
+      <c r="AT5" s="15">
         <f>SUM(AP4:AT4)</f>
         <v>0</v>
       </c>
-      <c r="AU5" s="14"/>
-      <c r="AV5" s="14"/>
-      <c r="AW5" s="14"/>
-      <c r="AX5" s="14"/>
-      <c r="AY5" s="16">
+      <c r="AU5" s="13"/>
+      <c r="AV5" s="13"/>
+      <c r="AW5" s="13"/>
+      <c r="AX5" s="13"/>
+      <c r="AY5" s="15">
         <f>SUM(AU4:AY4)</f>
         <v>0</v>
       </c>
@@ -1656,125 +1824,365 @@
       <c r="A6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="14">
         <f>SUM(B4:AY4)</f>
         <v>0</v>
       </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="28"/>
-      <c r="L6" s="28"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="28"/>
-      <c r="O6" s="28"/>
-      <c r="P6" s="28"/>
-      <c r="Q6" s="28"/>
-      <c r="R6" s="28"/>
-      <c r="S6" s="28"/>
-      <c r="T6" s="28"/>
-      <c r="U6" s="28"/>
-      <c r="V6" s="28"/>
-      <c r="W6" s="28"/>
-      <c r="X6" s="28"/>
-      <c r="Y6" s="28"/>
-      <c r="Z6" s="28"/>
-      <c r="AA6" s="28"/>
-      <c r="AB6" s="28"/>
-      <c r="AC6" s="28"/>
-      <c r="AD6" s="28"/>
-      <c r="AE6" s="28"/>
-      <c r="AF6" s="28"/>
-      <c r="AG6" s="28"/>
-      <c r="AH6" s="28"/>
-      <c r="AI6" s="28"/>
-      <c r="AJ6" s="28"/>
-      <c r="AK6" s="28"/>
-      <c r="AL6" s="28"/>
-      <c r="AM6" s="28"/>
-      <c r="AN6" s="28"/>
-      <c r="AO6" s="28"/>
-      <c r="AP6" s="28"/>
-      <c r="AQ6" s="28"/>
-      <c r="AR6" s="28"/>
-      <c r="AS6" s="28"/>
-      <c r="AT6" s="28"/>
-      <c r="AU6" s="28"/>
-      <c r="AV6" s="28"/>
-      <c r="AW6" s="28"/>
-      <c r="AX6" s="28"/>
-      <c r="AY6" s="28"/>
-    </row>
-    <row r="8" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A8" s="46" t="s">
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
+      <c r="Q6" s="26"/>
+      <c r="R6" s="26"/>
+      <c r="S6" s="26"/>
+      <c r="T6" s="26"/>
+      <c r="U6" s="26"/>
+      <c r="V6" s="26"/>
+      <c r="W6" s="26"/>
+      <c r="X6" s="26"/>
+      <c r="Y6" s="26"/>
+      <c r="Z6" s="26"/>
+      <c r="AA6" s="26"/>
+      <c r="AB6" s="26"/>
+      <c r="AC6" s="26"/>
+      <c r="AD6" s="26"/>
+      <c r="AE6" s="26"/>
+      <c r="AF6" s="26"/>
+      <c r="AG6" s="26"/>
+      <c r="AH6" s="26"/>
+      <c r="AI6" s="26"/>
+      <c r="AJ6" s="26"/>
+      <c r="AK6" s="26"/>
+      <c r="AL6" s="26"/>
+      <c r="AM6" s="26"/>
+      <c r="AN6" s="26"/>
+      <c r="AO6" s="26"/>
+      <c r="AP6" s="26"/>
+      <c r="AQ6" s="26"/>
+      <c r="AR6" s="26"/>
+      <c r="AS6" s="26"/>
+      <c r="AT6" s="26"/>
+      <c r="AU6" s="26"/>
+      <c r="AV6" s="26"/>
+      <c r="AW6" s="26"/>
+      <c r="AX6" s="26"/>
+      <c r="AY6" s="26"/>
+    </row>
+    <row r="8" spans="1:61" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="47"/>
-    </row>
-    <row r="9" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A9" s="46" t="s">
+      <c r="B8" s="55"/>
+      <c r="C8" s="58"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="60"/>
+      <c r="H8" s="63"/>
+      <c r="I8" s="59"/>
+      <c r="J8" s="59"/>
+      <c r="K8" s="60"/>
+      <c r="M8" s="58"/>
+      <c r="N8" s="59"/>
+      <c r="O8" s="59"/>
+      <c r="P8" s="60"/>
+      <c r="R8" s="63"/>
+      <c r="S8" s="59"/>
+      <c r="T8" s="59"/>
+      <c r="U8" s="60"/>
+      <c r="W8" s="58"/>
+      <c r="X8" s="59"/>
+      <c r="Y8" s="59"/>
+      <c r="Z8" s="60"/>
+      <c r="AB8" s="63"/>
+      <c r="AC8" s="59"/>
+      <c r="AD8" s="59"/>
+      <c r="AE8" s="60"/>
+      <c r="AG8" s="58"/>
+      <c r="AH8" s="59"/>
+      <c r="AI8" s="59"/>
+      <c r="AJ8" s="60"/>
+      <c r="AL8" s="63"/>
+      <c r="AM8" s="59"/>
+      <c r="AN8" s="59"/>
+      <c r="AO8" s="60"/>
+      <c r="AQ8" s="58"/>
+      <c r="AR8" s="59"/>
+      <c r="AS8" s="59"/>
+      <c r="AT8" s="60"/>
+      <c r="AV8" s="63"/>
+      <c r="AW8" s="59"/>
+      <c r="AX8" s="59"/>
+      <c r="AY8" s="60"/>
+    </row>
+    <row r="9" spans="1:61" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="47"/>
-    </row>
-    <row r="10" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A10" s="46" t="s">
+      <c r="B9" s="55"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="62"/>
+      <c r="H9" s="64"/>
+      <c r="I9" s="65"/>
+      <c r="J9" s="65"/>
+      <c r="K9" s="66"/>
+      <c r="M9" s="61"/>
+      <c r="N9" s="57"/>
+      <c r="O9" s="57"/>
+      <c r="P9" s="62"/>
+      <c r="R9" s="64"/>
+      <c r="S9" s="65"/>
+      <c r="T9" s="65"/>
+      <c r="U9" s="66"/>
+      <c r="W9" s="61"/>
+      <c r="X9" s="57"/>
+      <c r="Y9" s="57"/>
+      <c r="Z9" s="62"/>
+      <c r="AB9" s="64"/>
+      <c r="AC9" s="65"/>
+      <c r="AD9" s="65"/>
+      <c r="AE9" s="66"/>
+      <c r="AG9" s="61"/>
+      <c r="AH9" s="57"/>
+      <c r="AI9" s="57"/>
+      <c r="AJ9" s="62"/>
+      <c r="AL9" s="64"/>
+      <c r="AM9" s="65"/>
+      <c r="AN9" s="65"/>
+      <c r="AO9" s="66"/>
+      <c r="AQ9" s="61"/>
+      <c r="AR9" s="57"/>
+      <c r="AS9" s="57"/>
+      <c r="AT9" s="62"/>
+      <c r="AV9" s="64"/>
+      <c r="AW9" s="65"/>
+      <c r="AX9" s="65"/>
+      <c r="AY9" s="66"/>
+    </row>
+    <row r="10" spans="1:61" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="48"/>
-    </row>
-    <row r="11" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A11" s="46" t="s">
+      <c r="B10" s="56"/>
+      <c r="C10" s="58"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="59"/>
+      <c r="F10" s="60"/>
+      <c r="H10" s="63"/>
+      <c r="I10" s="59"/>
+      <c r="J10" s="59"/>
+      <c r="K10" s="60"/>
+      <c r="M10" s="58"/>
+      <c r="N10" s="59"/>
+      <c r="O10" s="59"/>
+      <c r="P10" s="60"/>
+      <c r="R10" s="63"/>
+      <c r="S10" s="59"/>
+      <c r="T10" s="59"/>
+      <c r="U10" s="60"/>
+      <c r="W10" s="58"/>
+      <c r="X10" s="59"/>
+      <c r="Y10" s="59"/>
+      <c r="Z10" s="60"/>
+      <c r="AB10" s="63"/>
+      <c r="AC10" s="59"/>
+      <c r="AD10" s="59"/>
+      <c r="AE10" s="60"/>
+      <c r="AG10" s="58"/>
+      <c r="AH10" s="59"/>
+      <c r="AI10" s="59"/>
+      <c r="AJ10" s="60"/>
+      <c r="AL10" s="63"/>
+      <c r="AM10" s="59"/>
+      <c r="AN10" s="59"/>
+      <c r="AO10" s="60"/>
+      <c r="AQ10" s="58"/>
+      <c r="AR10" s="59"/>
+      <c r="AS10" s="59"/>
+      <c r="AT10" s="60"/>
+      <c r="AV10" s="63"/>
+      <c r="AW10" s="59"/>
+      <c r="AX10" s="59"/>
+      <c r="AY10" s="60"/>
+    </row>
+    <row r="11" spans="1:61" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="47"/>
-    </row>
-    <row r="12" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="A12" s="46" t="s">
+      <c r="B11" s="55"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="60"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="59"/>
+      <c r="J11" s="59"/>
+      <c r="K11" s="60"/>
+      <c r="M11" s="58"/>
+      <c r="N11" s="59"/>
+      <c r="O11" s="59"/>
+      <c r="P11" s="60"/>
+      <c r="R11" s="63"/>
+      <c r="S11" s="59"/>
+      <c r="T11" s="59"/>
+      <c r="U11" s="60"/>
+      <c r="W11" s="58"/>
+      <c r="X11" s="59"/>
+      <c r="Y11" s="59"/>
+      <c r="Z11" s="60"/>
+      <c r="AB11" s="63"/>
+      <c r="AC11" s="59"/>
+      <c r="AD11" s="59"/>
+      <c r="AE11" s="60"/>
+      <c r="AG11" s="58"/>
+      <c r="AH11" s="59"/>
+      <c r="AI11" s="59"/>
+      <c r="AJ11" s="60"/>
+      <c r="AL11" s="63"/>
+      <c r="AM11" s="59"/>
+      <c r="AN11" s="59"/>
+      <c r="AO11" s="60"/>
+      <c r="AQ11" s="58"/>
+      <c r="AR11" s="59"/>
+      <c r="AS11" s="59"/>
+      <c r="AT11" s="60"/>
+      <c r="AV11" s="63"/>
+      <c r="AW11" s="59"/>
+      <c r="AX11" s="59"/>
+      <c r="AY11" s="60"/>
+    </row>
+    <row r="12" spans="1:61" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="49"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="60"/>
+      <c r="H12" s="63"/>
+      <c r="I12" s="59"/>
+      <c r="J12" s="59"/>
+      <c r="K12" s="60"/>
+      <c r="M12" s="58"/>
+      <c r="N12" s="59"/>
+      <c r="O12" s="59"/>
+      <c r="P12" s="60"/>
+      <c r="R12" s="63"/>
+      <c r="S12" s="59"/>
+      <c r="T12" s="59"/>
+      <c r="U12" s="60"/>
+      <c r="W12" s="58"/>
+      <c r="X12" s="59"/>
+      <c r="Y12" s="59"/>
+      <c r="Z12" s="60"/>
+      <c r="AB12" s="63"/>
+      <c r="AC12" s="59"/>
+      <c r="AD12" s="59"/>
+      <c r="AE12" s="60"/>
+      <c r="AG12" s="58"/>
+      <c r="AH12" s="59"/>
+      <c r="AI12" s="59"/>
+      <c r="AJ12" s="60"/>
+      <c r="AL12" s="63"/>
+      <c r="AM12" s="59"/>
+      <c r="AN12" s="59"/>
+      <c r="AO12" s="60"/>
+      <c r="AQ12" s="58"/>
+      <c r="AR12" s="59"/>
+      <c r="AS12" s="59"/>
+      <c r="AT12" s="60"/>
+      <c r="AV12" s="63"/>
+      <c r="AW12" s="59"/>
+      <c r="AX12" s="59"/>
+      <c r="AY12" s="60"/>
     </row>
     <row r="13" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="B13" s="7"/>
+      <c r="B13" s="6"/>
     </row>
     <row r="14" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="B14" s="7"/>
+      <c r="B14" s="6"/>
     </row>
     <row r="15" spans="1:61" x14ac:dyDescent="0.2">
-      <c r="B15" s="7"/>
+      <c r="B15" s="6"/>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" s="7"/>
+      <c r="B17" s="6"/>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18" s="7"/>
+      <c r="B18" s="6"/>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B19" s="7"/>
+      <c r="B19" s="6"/>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B22" s="7"/>
+      <c r="B22" s="6"/>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B23" s="7"/>
+      <c r="B23" s="6"/>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B24" s="7"/>
+      <c r="B24" s="6"/>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B25" s="7"/>
+      <c r="B25" s="6"/>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B26" s="7"/>
+      <c r="B26" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="45">
+    <mergeCell ref="AG12:AJ12"/>
+    <mergeCell ref="AL12:AO12"/>
+    <mergeCell ref="AQ8:AT8"/>
+    <mergeCell ref="AV8:AY8"/>
+    <mergeCell ref="AQ10:AT10"/>
+    <mergeCell ref="AV10:AY10"/>
+    <mergeCell ref="AQ11:AT11"/>
+    <mergeCell ref="AV11:AY11"/>
+    <mergeCell ref="AQ12:AT12"/>
+    <mergeCell ref="AV12:AY12"/>
+    <mergeCell ref="AG8:AJ8"/>
+    <mergeCell ref="AL8:AO8"/>
+    <mergeCell ref="AG10:AJ10"/>
+    <mergeCell ref="AL10:AO10"/>
+    <mergeCell ref="AG11:AJ11"/>
+    <mergeCell ref="AL11:AO11"/>
+    <mergeCell ref="M12:P12"/>
+    <mergeCell ref="R12:U12"/>
+    <mergeCell ref="W8:Z8"/>
+    <mergeCell ref="AB8:AE8"/>
+    <mergeCell ref="W10:Z10"/>
+    <mergeCell ref="AB10:AE10"/>
+    <mergeCell ref="W11:Z11"/>
+    <mergeCell ref="AB11:AE11"/>
+    <mergeCell ref="W12:Z12"/>
+    <mergeCell ref="AB12:AE12"/>
+    <mergeCell ref="M8:P8"/>
+    <mergeCell ref="R8:U8"/>
+    <mergeCell ref="M10:P10"/>
+    <mergeCell ref="R10:U10"/>
+    <mergeCell ref="M11:P11"/>
+    <mergeCell ref="R11:U11"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="H12:K12"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
@@ -1782,6 +2190,7 @@
     <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1791,7 +2200,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1802,70 +2211,70 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B2" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="23" t="s">
+      <c r="B2" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="23" t="s">
+      <c r="I2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="26" t="s">
+      <c r="J2" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="23" t="s">
+      <c r="K2" s="22" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="13"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="12"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="27">
+      <c r="B5" s="54">
         <f>SUM(B3:K3)</f>
         <v>0</v>
       </c>
@@ -1881,7 +2290,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1895,76 +2304,76 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B2" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="23" t="s">
+      <c r="B2" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E2" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="23" t="s">
+      <c r="G2" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="23" t="s">
+      <c r="I2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="26" t="s">
+      <c r="J2" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="23" t="s">
+      <c r="K2" s="22" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="13"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="12"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="14"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="31" t="s">
+      <c r="A5" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="27">
+      <c r="B5" s="54">
         <f>SUM(B3:K3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="10"/>
+      <c r="A6" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated term project rubric and weekly report sspreadsheets
</commit_message>
<xml_diff>
--- a/CS297-WeeklyIndividualReport.xlsx
+++ b/CS297-WeeklyIndividualReport.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS297-CourseMaterials/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DataCard/Repos/CS297-Repos/CS297-CourseMaterials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61971F4C-094F-BA44-918F-38B1BC66FC5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39216098-BDD9-9148-88D7-18336B5C5830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="26240" windowHeight="15500" xr2:uid="{AF13BEBC-A70C-7746-A217-C0986067414B}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="26240" windowHeight="15460" activeTab="4" xr2:uid="{AF13BEBC-A70C-7746-A217-C0986067414B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Attendence" sheetId="1" r:id="rId1"/>
+    <sheet name="Attendance" sheetId="1" r:id="rId1"/>
     <sheet name="Hours" sheetId="2" r:id="rId2"/>
     <sheet name="PRs" sheetId="3" r:id="rId3"/>
-    <sheet name="User Stories" sheetId="4" r:id="rId4"/>
+    <sheet name="Story Points" sheetId="4" r:id="rId4"/>
+    <sheet name="Score" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="62">
   <si>
     <t>Week 1</t>
   </si>
@@ -152,9 +153,6 @@
     <t>Number of PRs created per week</t>
   </si>
   <si>
-    <t>CS297 Capstone, spring 2025</t>
-  </si>
-  <si>
     <t>Subtotal</t>
   </si>
   <si>
@@ -170,9 +168,6 @@
     <t>No meeting</t>
   </si>
   <si>
-    <t>Number of task user story points completed each week</t>
-  </si>
-  <si>
     <t>Is your work up to date on Jira?</t>
   </si>
   <si>
@@ -186,13 +181,58 @@
   </si>
   <si>
     <t>What is your assessment of your progress this week?</t>
+  </si>
+  <si>
+    <t>Team Participation Score</t>
+  </si>
+  <si>
+    <t>You did a good job of contributing to the success your team's project! Here is the participation grade breakdown:</t>
+  </si>
+  <si>
+    <t>Possible</t>
+  </si>
+  <si>
+    <t>Points</t>
+  </si>
+  <si>
+    <t>Stats</t>
+  </si>
+  <si>
+    <t>Participation with your team</t>
+  </si>
+  <si>
+    <t>Git pull requests (1 per week)</t>
+  </si>
+  <si>
+    <t>Sprint meeting attendance (3 per sprint)</t>
+  </si>
+  <si>
+    <t>Daily Stand-ups (4 per week)</t>
+  </si>
+  <si>
+    <t>Team work sessions (4 per week)</t>
+  </si>
+  <si>
+    <t>Hours worked (12 per week)</t>
+  </si>
+  <si>
+    <t>Total (100 maximum)</t>
+  </si>
+  <si>
+    <t>User story hours/points completed (8 per week)</t>
+  </si>
+  <si>
+    <t>CS297 Capstone, spring 2026</t>
+  </si>
+  <si>
+    <t>User story (issue) points completed each week</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -221,6 +261,14 @@
       <color rgb="FF000000"/>
       <name val="Verdana"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="12">
@@ -508,7 +556,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -560,21 +608,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="2" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -601,27 +634,41 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -939,8 +986,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:Q24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -953,41 +1000,41 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="B1" s="1"/>
       <c r="D1" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="35"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
       <c r="H1" s="1"/>
       <c r="I1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="J1" s="38"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="36"/>
+        <v>38</v>
+      </c>
+      <c r="J1" s="57"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="55"/>
     </row>
     <row r="2" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="49"/>
+      <c r="A2" s="42"/>
       <c r="D2" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="37"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
       <c r="I2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J2" s="38"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="36"/>
+        <v>39</v>
+      </c>
+      <c r="J2" s="57"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="55"/>
       <c r="Q2" s="2"/>
     </row>
     <row r="3" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="50"/>
+      <c r="A3" s="43"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
@@ -999,54 +1046,54 @@
       <c r="Q3" s="2"/>
     </row>
     <row r="4" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="51"/>
+      <c r="A4" s="44"/>
       <c r="B4" s="29"/>
       <c r="C4" s="30"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="43"/>
-      <c r="L4" s="43"/>
-      <c r="M4" s="44"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="37"/>
       <c r="N4" s="5"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
     </row>
     <row r="5" spans="1:17" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="52"/>
-      <c r="D5" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="46" t="s">
+      <c r="A5" s="45"/>
+      <c r="D5" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="47" t="s">
+      <c r="F5" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="47" t="s">
+      <c r="G5" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="47" t="s">
+      <c r="H5" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="47" t="s">
+      <c r="I5" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="47" t="s">
+      <c r="J5" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="47" t="s">
+      <c r="K5" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="47" t="s">
+      <c r="L5" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="48" t="s">
+      <c r="M5" s="41" t="s">
         <v>13</v>
       </c>
       <c r="N5" s="5"/>
@@ -1057,7 +1104,7 @@
       <c r="Q5" s="2"/>
     </row>
     <row r="6" spans="1:17" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="33" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="17"/>
@@ -1073,7 +1120,7 @@
       <c r="L6" s="31"/>
       <c r="M6" s="32"/>
       <c r="N6" s="10"/>
-      <c r="O6" s="53">
+      <c r="O6" s="46">
         <f>COUNTIF(D6:M6, "P") + ROUND(0.7*COUNTIF(D6:M6, "L"),0)</f>
         <v>0</v>
       </c>
@@ -1097,7 +1144,7 @@
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
       <c r="N7" s="10"/>
-      <c r="O7" s="53">
+      <c r="O7" s="46">
         <f t="shared" ref="O7:O18" si="0">COUNTIF(D7:M7, "P") + ROUND(0.7*COUNTIF(D7:M7, "L"),0)</f>
         <v>0</v>
       </c>
@@ -1120,7 +1167,7 @@
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
       <c r="N8" s="10"/>
-      <c r="O8" s="53">
+      <c r="O8" s="46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1142,7 +1189,7 @@
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
       <c r="N9" s="10"/>
-      <c r="O9" s="53">
+      <c r="O9" s="46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1164,7 +1211,7 @@
       <c r="L10" s="8"/>
       <c r="M10" s="8"/>
       <c r="N10" s="10"/>
-      <c r="O10" s="53">
+      <c r="O10" s="46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1186,7 +1233,7 @@
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
       <c r="N11" s="10"/>
-      <c r="O11" s="53">
+      <c r="O11" s="46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1210,7 +1257,7 @@
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
       <c r="N12" s="10"/>
-      <c r="O12" s="53">
+      <c r="O12" s="46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1232,7 +1279,7 @@
       <c r="L13" s="7"/>
       <c r="M13" s="7"/>
       <c r="N13" s="10"/>
-      <c r="O13" s="53">
+      <c r="O13" s="46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1254,7 +1301,7 @@
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
       <c r="N14" s="10"/>
-      <c r="O14" s="53">
+      <c r="O14" s="46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1276,7 +1323,7 @@
       <c r="L15" s="7"/>
       <c r="M15" s="7"/>
       <c r="N15" s="10"/>
-      <c r="O15" s="53">
+      <c r="O15" s="46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1298,7 +1345,7 @@
       <c r="L16" s="7"/>
       <c r="M16" s="7"/>
       <c r="N16" s="10"/>
-      <c r="O16" s="53">
+      <c r="O16" s="46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1320,7 +1367,7 @@
       <c r="L17" s="10"/>
       <c r="M17" s="8"/>
       <c r="N17" s="10"/>
-      <c r="O17" s="53">
+      <c r="O17" s="46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1342,7 +1389,7 @@
       <c r="L18" s="10"/>
       <c r="M18" s="7"/>
       <c r="N18" s="10"/>
-      <c r="O18" s="53">
+      <c r="O18" s="46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1386,10 +1433,10 @@
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" t="s">
         <v>41</v>
-      </c>
-      <c r="D24" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1737,7 +1784,7 @@
     </row>
     <row r="5" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="10"/>
       <c r="C5" s="13"/>
@@ -1879,234 +1926,234 @@
       <c r="AY6" s="26"/>
     </row>
     <row r="8" spans="1:61" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="63" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="64"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="61"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="60"/>
+      <c r="J8" s="60"/>
+      <c r="K8" s="61"/>
+      <c r="M8" s="59"/>
+      <c r="N8" s="60"/>
+      <c r="O8" s="60"/>
+      <c r="P8" s="61"/>
+      <c r="R8" s="62"/>
+      <c r="S8" s="60"/>
+      <c r="T8" s="60"/>
+      <c r="U8" s="61"/>
+      <c r="W8" s="59"/>
+      <c r="X8" s="60"/>
+      <c r="Y8" s="60"/>
+      <c r="Z8" s="61"/>
+      <c r="AB8" s="62"/>
+      <c r="AC8" s="60"/>
+      <c r="AD8" s="60"/>
+      <c r="AE8" s="61"/>
+      <c r="AG8" s="59"/>
+      <c r="AH8" s="60"/>
+      <c r="AI8" s="60"/>
+      <c r="AJ8" s="61"/>
+      <c r="AL8" s="62"/>
+      <c r="AM8" s="60"/>
+      <c r="AN8" s="60"/>
+      <c r="AO8" s="61"/>
+      <c r="AQ8" s="59"/>
+      <c r="AR8" s="60"/>
+      <c r="AS8" s="60"/>
+      <c r="AT8" s="61"/>
+      <c r="AV8" s="62"/>
+      <c r="AW8" s="60"/>
+      <c r="AX8" s="60"/>
+      <c r="AY8" s="61"/>
+    </row>
+    <row r="9" spans="1:61" ht="38" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="63" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="64"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="48"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="50"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="52"/>
+      <c r="K9" s="53"/>
+      <c r="M9" s="49"/>
+      <c r="N9" s="48"/>
+      <c r="O9" s="48"/>
+      <c r="P9" s="50"/>
+      <c r="R9" s="51"/>
+      <c r="S9" s="52"/>
+      <c r="T9" s="52"/>
+      <c r="U9" s="53"/>
+      <c r="W9" s="49"/>
+      <c r="X9" s="48"/>
+      <c r="Y9" s="48"/>
+      <c r="Z9" s="50"/>
+      <c r="AB9" s="51"/>
+      <c r="AC9" s="52"/>
+      <c r="AD9" s="52"/>
+      <c r="AE9" s="53"/>
+      <c r="AG9" s="49"/>
+      <c r="AH9" s="48"/>
+      <c r="AI9" s="48"/>
+      <c r="AJ9" s="50"/>
+      <c r="AL9" s="51"/>
+      <c r="AM9" s="52"/>
+      <c r="AN9" s="52"/>
+      <c r="AO9" s="53"/>
+      <c r="AQ9" s="49"/>
+      <c r="AR9" s="48"/>
+      <c r="AS9" s="48"/>
+      <c r="AT9" s="50"/>
+      <c r="AV9" s="51"/>
+      <c r="AW9" s="52"/>
+      <c r="AX9" s="52"/>
+      <c r="AY9" s="53"/>
+    </row>
+    <row r="10" spans="1:61" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="55"/>
-      <c r="C8" s="58"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="60"/>
-      <c r="H8" s="63"/>
-      <c r="I8" s="59"/>
-      <c r="J8" s="59"/>
-      <c r="K8" s="60"/>
-      <c r="M8" s="58"/>
-      <c r="N8" s="59"/>
-      <c r="O8" s="59"/>
-      <c r="P8" s="60"/>
-      <c r="R8" s="63"/>
-      <c r="S8" s="59"/>
-      <c r="T8" s="59"/>
-      <c r="U8" s="60"/>
-      <c r="W8" s="58"/>
-      <c r="X8" s="59"/>
-      <c r="Y8" s="59"/>
-      <c r="Z8" s="60"/>
-      <c r="AB8" s="63"/>
-      <c r="AC8" s="59"/>
-      <c r="AD8" s="59"/>
-      <c r="AE8" s="60"/>
-      <c r="AG8" s="58"/>
-      <c r="AH8" s="59"/>
-      <c r="AI8" s="59"/>
-      <c r="AJ8" s="60"/>
-      <c r="AL8" s="63"/>
-      <c r="AM8" s="59"/>
-      <c r="AN8" s="59"/>
-      <c r="AO8" s="60"/>
-      <c r="AQ8" s="58"/>
-      <c r="AR8" s="59"/>
-      <c r="AS8" s="59"/>
-      <c r="AT8" s="60"/>
-      <c r="AV8" s="63"/>
-      <c r="AW8" s="59"/>
-      <c r="AX8" s="59"/>
-      <c r="AY8" s="60"/>
-    </row>
-    <row r="9" spans="1:61" ht="38" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" s="55"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="62"/>
-      <c r="H9" s="64"/>
-      <c r="I9" s="65"/>
-      <c r="J9" s="65"/>
-      <c r="K9" s="66"/>
-      <c r="M9" s="61"/>
-      <c r="N9" s="57"/>
-      <c r="O9" s="57"/>
-      <c r="P9" s="62"/>
-      <c r="R9" s="64"/>
-      <c r="S9" s="65"/>
-      <c r="T9" s="65"/>
-      <c r="U9" s="66"/>
-      <c r="W9" s="61"/>
-      <c r="X9" s="57"/>
-      <c r="Y9" s="57"/>
-      <c r="Z9" s="62"/>
-      <c r="AB9" s="64"/>
-      <c r="AC9" s="65"/>
-      <c r="AD9" s="65"/>
-      <c r="AE9" s="66"/>
-      <c r="AG9" s="61"/>
-      <c r="AH9" s="57"/>
-      <c r="AI9" s="57"/>
-      <c r="AJ9" s="62"/>
-      <c r="AL9" s="64"/>
-      <c r="AM9" s="65"/>
-      <c r="AN9" s="65"/>
-      <c r="AO9" s="66"/>
-      <c r="AQ9" s="61"/>
-      <c r="AR9" s="57"/>
-      <c r="AS9" s="57"/>
-      <c r="AT9" s="62"/>
-      <c r="AV9" s="64"/>
-      <c r="AW9" s="65"/>
-      <c r="AX9" s="65"/>
-      <c r="AY9" s="66"/>
-    </row>
-    <row r="10" spans="1:61" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="56"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="59"/>
-      <c r="E10" s="59"/>
-      <c r="F10" s="60"/>
-      <c r="H10" s="63"/>
-      <c r="I10" s="59"/>
-      <c r="J10" s="59"/>
-      <c r="K10" s="60"/>
-      <c r="M10" s="58"/>
-      <c r="N10" s="59"/>
-      <c r="O10" s="59"/>
-      <c r="P10" s="60"/>
-      <c r="R10" s="63"/>
-      <c r="S10" s="59"/>
-      <c r="T10" s="59"/>
-      <c r="U10" s="60"/>
-      <c r="W10" s="58"/>
-      <c r="X10" s="59"/>
-      <c r="Y10" s="59"/>
-      <c r="Z10" s="60"/>
-      <c r="AB10" s="63"/>
-      <c r="AC10" s="59"/>
-      <c r="AD10" s="59"/>
-      <c r="AE10" s="60"/>
-      <c r="AG10" s="58"/>
-      <c r="AH10" s="59"/>
-      <c r="AI10" s="59"/>
-      <c r="AJ10" s="60"/>
-      <c r="AL10" s="63"/>
-      <c r="AM10" s="59"/>
-      <c r="AN10" s="59"/>
-      <c r="AO10" s="60"/>
-      <c r="AQ10" s="58"/>
-      <c r="AR10" s="59"/>
-      <c r="AS10" s="59"/>
-      <c r="AT10" s="60"/>
-      <c r="AV10" s="63"/>
-      <c r="AW10" s="59"/>
-      <c r="AX10" s="59"/>
-      <c r="AY10" s="60"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="61"/>
+      <c r="H10" s="62"/>
+      <c r="I10" s="60"/>
+      <c r="J10" s="60"/>
+      <c r="K10" s="61"/>
+      <c r="M10" s="59"/>
+      <c r="N10" s="60"/>
+      <c r="O10" s="60"/>
+      <c r="P10" s="61"/>
+      <c r="R10" s="62"/>
+      <c r="S10" s="60"/>
+      <c r="T10" s="60"/>
+      <c r="U10" s="61"/>
+      <c r="W10" s="59"/>
+      <c r="X10" s="60"/>
+      <c r="Y10" s="60"/>
+      <c r="Z10" s="61"/>
+      <c r="AB10" s="62"/>
+      <c r="AC10" s="60"/>
+      <c r="AD10" s="60"/>
+      <c r="AE10" s="61"/>
+      <c r="AG10" s="59"/>
+      <c r="AH10" s="60"/>
+      <c r="AI10" s="60"/>
+      <c r="AJ10" s="61"/>
+      <c r="AL10" s="62"/>
+      <c r="AM10" s="60"/>
+      <c r="AN10" s="60"/>
+      <c r="AO10" s="61"/>
+      <c r="AQ10" s="59"/>
+      <c r="AR10" s="60"/>
+      <c r="AS10" s="60"/>
+      <c r="AT10" s="61"/>
+      <c r="AV10" s="62"/>
+      <c r="AW10" s="60"/>
+      <c r="AX10" s="60"/>
+      <c r="AY10" s="61"/>
     </row>
     <row r="11" spans="1:61" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="63" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="64"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="61"/>
+      <c r="H11" s="62"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="60"/>
+      <c r="K11" s="61"/>
+      <c r="M11" s="59"/>
+      <c r="N11" s="60"/>
+      <c r="O11" s="60"/>
+      <c r="P11" s="61"/>
+      <c r="R11" s="62"/>
+      <c r="S11" s="60"/>
+      <c r="T11" s="60"/>
+      <c r="U11" s="61"/>
+      <c r="W11" s="59"/>
+      <c r="X11" s="60"/>
+      <c r="Y11" s="60"/>
+      <c r="Z11" s="61"/>
+      <c r="AB11" s="62"/>
+      <c r="AC11" s="60"/>
+      <c r="AD11" s="60"/>
+      <c r="AE11" s="61"/>
+      <c r="AG11" s="59"/>
+      <c r="AH11" s="60"/>
+      <c r="AI11" s="60"/>
+      <c r="AJ11" s="61"/>
+      <c r="AL11" s="62"/>
+      <c r="AM11" s="60"/>
+      <c r="AN11" s="60"/>
+      <c r="AO11" s="61"/>
+      <c r="AQ11" s="59"/>
+      <c r="AR11" s="60"/>
+      <c r="AS11" s="60"/>
+      <c r="AT11" s="61"/>
+      <c r="AV11" s="62"/>
+      <c r="AW11" s="60"/>
+      <c r="AX11" s="60"/>
+      <c r="AY11" s="61"/>
+    </row>
+    <row r="12" spans="1:61" ht="34" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="63" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="55"/>
-      <c r="C11" s="58"/>
-      <c r="D11" s="59"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="60"/>
-      <c r="H11" s="63"/>
-      <c r="I11" s="59"/>
-      <c r="J11" s="59"/>
-      <c r="K11" s="60"/>
-      <c r="M11" s="58"/>
-      <c r="N11" s="59"/>
-      <c r="O11" s="59"/>
-      <c r="P11" s="60"/>
-      <c r="R11" s="63"/>
-      <c r="S11" s="59"/>
-      <c r="T11" s="59"/>
-      <c r="U11" s="60"/>
-      <c r="W11" s="58"/>
-      <c r="X11" s="59"/>
-      <c r="Y11" s="59"/>
-      <c r="Z11" s="60"/>
-      <c r="AB11" s="63"/>
-      <c r="AC11" s="59"/>
-      <c r="AD11" s="59"/>
-      <c r="AE11" s="60"/>
-      <c r="AG11" s="58"/>
-      <c r="AH11" s="59"/>
-      <c r="AI11" s="59"/>
-      <c r="AJ11" s="60"/>
-      <c r="AL11" s="63"/>
-      <c r="AM11" s="59"/>
-      <c r="AN11" s="59"/>
-      <c r="AO11" s="60"/>
-      <c r="AQ11" s="58"/>
-      <c r="AR11" s="59"/>
-      <c r="AS11" s="59"/>
-      <c r="AT11" s="60"/>
-      <c r="AV11" s="63"/>
-      <c r="AW11" s="59"/>
-      <c r="AX11" s="59"/>
-      <c r="AY11" s="60"/>
-    </row>
-    <row r="12" spans="1:61" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12" s="34"/>
-      <c r="C12" s="58"/>
-      <c r="D12" s="59"/>
-      <c r="E12" s="59"/>
-      <c r="F12" s="60"/>
-      <c r="H12" s="63"/>
-      <c r="I12" s="59"/>
-      <c r="J12" s="59"/>
-      <c r="K12" s="60"/>
-      <c r="M12" s="58"/>
-      <c r="N12" s="59"/>
-      <c r="O12" s="59"/>
-      <c r="P12" s="60"/>
-      <c r="R12" s="63"/>
-      <c r="S12" s="59"/>
-      <c r="T12" s="59"/>
-      <c r="U12" s="60"/>
-      <c r="W12" s="58"/>
-      <c r="X12" s="59"/>
-      <c r="Y12" s="59"/>
-      <c r="Z12" s="60"/>
-      <c r="AB12" s="63"/>
-      <c r="AC12" s="59"/>
-      <c r="AD12" s="59"/>
-      <c r="AE12" s="60"/>
-      <c r="AG12" s="58"/>
-      <c r="AH12" s="59"/>
-      <c r="AI12" s="59"/>
-      <c r="AJ12" s="60"/>
-      <c r="AL12" s="63"/>
-      <c r="AM12" s="59"/>
-      <c r="AN12" s="59"/>
-      <c r="AO12" s="60"/>
-      <c r="AQ12" s="58"/>
-      <c r="AR12" s="59"/>
-      <c r="AS12" s="59"/>
-      <c r="AT12" s="60"/>
-      <c r="AV12" s="63"/>
-      <c r="AW12" s="59"/>
-      <c r="AX12" s="59"/>
-      <c r="AY12" s="60"/>
+      <c r="B12" s="64"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="60"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="61"/>
+      <c r="H12" s="62"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="60"/>
+      <c r="K12" s="61"/>
+      <c r="M12" s="59"/>
+      <c r="N12" s="60"/>
+      <c r="O12" s="60"/>
+      <c r="P12" s="61"/>
+      <c r="R12" s="62"/>
+      <c r="S12" s="60"/>
+      <c r="T12" s="60"/>
+      <c r="U12" s="61"/>
+      <c r="W12" s="59"/>
+      <c r="X12" s="60"/>
+      <c r="Y12" s="60"/>
+      <c r="Z12" s="61"/>
+      <c r="AB12" s="62"/>
+      <c r="AC12" s="60"/>
+      <c r="AD12" s="60"/>
+      <c r="AE12" s="61"/>
+      <c r="AG12" s="59"/>
+      <c r="AH12" s="60"/>
+      <c r="AI12" s="60"/>
+      <c r="AJ12" s="61"/>
+      <c r="AL12" s="62"/>
+      <c r="AM12" s="60"/>
+      <c r="AN12" s="60"/>
+      <c r="AO12" s="61"/>
+      <c r="AQ12" s="59"/>
+      <c r="AR12" s="60"/>
+      <c r="AS12" s="60"/>
+      <c r="AT12" s="61"/>
+      <c r="AV12" s="62"/>
+      <c r="AW12" s="60"/>
+      <c r="AX12" s="60"/>
+      <c r="AY12" s="61"/>
     </row>
     <row r="13" spans="1:61" x14ac:dyDescent="0.2">
       <c r="B13" s="6"/>
@@ -2143,6 +2190,35 @@
     </row>
   </sheetData>
   <mergeCells count="45">
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="H8:K8"/>
+    <mergeCell ref="H10:K10"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="H12:K12"/>
+    <mergeCell ref="M12:P12"/>
+    <mergeCell ref="R12:U12"/>
+    <mergeCell ref="W8:Z8"/>
+    <mergeCell ref="AB8:AE8"/>
+    <mergeCell ref="W10:Z10"/>
+    <mergeCell ref="AB10:AE10"/>
+    <mergeCell ref="W11:Z11"/>
+    <mergeCell ref="AB11:AE11"/>
+    <mergeCell ref="W12:Z12"/>
+    <mergeCell ref="AB12:AE12"/>
+    <mergeCell ref="M8:P8"/>
+    <mergeCell ref="R8:U8"/>
+    <mergeCell ref="M10:P10"/>
+    <mergeCell ref="R10:U10"/>
+    <mergeCell ref="M11:P11"/>
+    <mergeCell ref="R11:U11"/>
     <mergeCell ref="AG12:AJ12"/>
     <mergeCell ref="AL12:AO12"/>
     <mergeCell ref="AQ8:AT8"/>
@@ -2159,35 +2235,6 @@
     <mergeCell ref="AL10:AO10"/>
     <mergeCell ref="AG11:AJ11"/>
     <mergeCell ref="AL11:AO11"/>
-    <mergeCell ref="M12:P12"/>
-    <mergeCell ref="R12:U12"/>
-    <mergeCell ref="W8:Z8"/>
-    <mergeCell ref="AB8:AE8"/>
-    <mergeCell ref="W10:Z10"/>
-    <mergeCell ref="AB10:AE10"/>
-    <mergeCell ref="W11:Z11"/>
-    <mergeCell ref="AB11:AE11"/>
-    <mergeCell ref="W12:Z12"/>
-    <mergeCell ref="AB12:AE12"/>
-    <mergeCell ref="M8:P8"/>
-    <mergeCell ref="R8:U8"/>
-    <mergeCell ref="M10:P10"/>
-    <mergeCell ref="R10:U10"/>
-    <mergeCell ref="M11:P11"/>
-    <mergeCell ref="R11:U11"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="H10:K10"/>
-    <mergeCell ref="H11:K11"/>
-    <mergeCell ref="H12:K12"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2274,7 +2321,7 @@
       <c r="A5" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="54">
+      <c r="B5" s="47">
         <f>SUM(B3:K3)</f>
         <v>0</v>
       </c>
@@ -2290,7 +2337,7 @@
   <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2300,7 +2347,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -2367,13 +2414,171 @@
       <c r="A5" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="54">
+      <c r="B5" s="47">
         <f>SUM(B3:K3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F921E1A-DF40-114B-BEAE-ACBF7BD4053C}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="30" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="30"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="67" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="67" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="67" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="67" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>20</v>
+      </c>
+      <c r="B6" s="66">
+        <f>MAX(20,C6*2)</f>
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <f>PRs!$B$5</f>
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>30</v>
+      </c>
+      <c r="B7" s="66">
+        <f>C7*3/8</f>
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <f>'Story Points'!$B$5</f>
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>10</v>
+      </c>
+      <c r="B8" s="66">
+        <f>C8*2/3</f>
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <f>Attendance!$O$6 +Attendance!$O$17+Attendance!$O$18</f>
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>10</v>
+      </c>
+      <c r="B9" s="66">
+        <f>C9/4</f>
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <f>SUM(Attendance!$O$7       : Attendance!$O$11)</f>
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" s="66">
+        <f>C10/4</f>
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <f>SUM(Attendance!$O$12       : Attendance!$O$16)</f>
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>20</v>
+      </c>
+      <c r="B11" s="66">
+        <f>C11/6</f>
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <f>Hours!$B$6</f>
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <f>SUM(A6:A11)</f>
+        <v>100</v>
+      </c>
+      <c r="B13" s="66">
+        <f>SUM(B6:B11)</f>
+        <v>20</v>
+      </c>
+      <c r="E13" t="s">
+        <v>58</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>